<commit_message>
new data file and color corrections added
</commit_message>
<xml_diff>
--- a/data/metadata_final.xlsx
+++ b/data/metadata_final.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Apps\covid-act\public\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ADD316C-BA92-41DC-9497-5C46CAB94380}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EB551DB-E06B-433C-9DCB-3E27CBE12A91}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A6CE5D30-78AA-430F-9DE7-4D01A36A5353}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="68">
   <si>
     <t>id</t>
   </si>
@@ -143,30 +143,12 @@
     <t>comments</t>
   </si>
   <si>
-    <t>level_dir</t>
-  </si>
-  <si>
     <t>asc</t>
   </si>
   <si>
     <t>desc</t>
   </si>
   <si>
-    <t>level_1</t>
-  </si>
-  <si>
-    <t>level_2</t>
-  </si>
-  <si>
-    <t>level_3</t>
-  </si>
-  <si>
-    <t>level_4</t>
-  </si>
-  <si>
-    <t>level_value</t>
-  </si>
-  <si>
     <t>value</t>
   </si>
   <si>
@@ -234,6 +216,27 @@
   </si>
   <si>
     <t>%</t>
+  </si>
+  <si>
+    <t>risk_dir</t>
+  </si>
+  <si>
+    <t>risk_1</t>
+  </si>
+  <si>
+    <t>risk_2</t>
+  </si>
+  <si>
+    <t>risk_3</t>
+  </si>
+  <si>
+    <t>risk_4</t>
+  </si>
+  <si>
+    <t>risk_5</t>
+  </si>
+  <si>
+    <t>risk_level</t>
   </si>
 </sst>
 </file>
@@ -585,20 +588,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{272B52F7-A458-4327-BA6F-D3011567919B}">
-  <dimension ref="A1:U11"/>
+  <dimension ref="A1:V11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="A22" sqref="A1:XFD22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C1" t="s">
         <v>11</v>
@@ -616,54 +619,57 @@
         <v>35</v>
       </c>
       <c r="H1" t="s">
-        <v>36</v>
+        <v>61</v>
       </c>
       <c r="I1" t="s">
+        <v>62</v>
+      </c>
+      <c r="J1" t="s">
+        <v>63</v>
+      </c>
+      <c r="K1" t="s">
+        <v>64</v>
+      </c>
+      <c r="L1" t="s">
+        <v>65</v>
+      </c>
+      <c r="M1" t="s">
+        <v>66</v>
+      </c>
+      <c r="N1" t="s">
+        <v>67</v>
+      </c>
+      <c r="O1" t="s">
+        <v>38</v>
+      </c>
+      <c r="P1" t="s">
         <v>39</v>
       </c>
-      <c r="J1" t="s">
+      <c r="Q1" t="s">
         <v>40</v>
       </c>
-      <c r="K1" t="s">
+      <c r="R1" t="s">
         <v>41</v>
       </c>
-      <c r="L1" t="s">
+      <c r="S1" t="s">
         <v>42</v>
       </c>
-      <c r="M1" t="s">
+      <c r="T1" t="s">
         <v>43</v>
       </c>
-      <c r="N1" t="s">
+      <c r="U1" t="s">
         <v>44</v>
       </c>
-      <c r="O1" t="s">
-        <v>45</v>
-      </c>
-      <c r="P1" t="s">
+      <c r="V1" t="s">
         <v>46</v>
       </c>
-      <c r="Q1" t="s">
-        <v>47</v>
-      </c>
-      <c r="R1" t="s">
-        <v>48</v>
-      </c>
-      <c r="S1" t="s">
-        <v>49</v>
-      </c>
-      <c r="T1" t="s">
-        <v>50</v>
-      </c>
-      <c r="U1" t="s">
-        <v>52</v>
-      </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C2" t="s">
         <v>12</v>
@@ -678,7 +684,7 @@
         <v>31</v>
       </c>
       <c r="H2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I2">
         <v>1</v>
@@ -687,42 +693,45 @@
         <v>25</v>
       </c>
       <c r="K2">
+        <v>50</v>
+      </c>
+      <c r="L2">
         <v>75</v>
       </c>
-      <c r="M2">
+      <c r="N2">
         <v>4</v>
       </c>
-      <c r="N2">
+      <c r="O2">
         <v>106</v>
       </c>
-      <c r="O2">
+      <c r="P2">
         <v>193</v>
       </c>
-      <c r="P2">
+      <c r="Q2">
         <v>20507</v>
       </c>
-      <c r="Q2">
+      <c r="R2">
         <v>106</v>
       </c>
-      <c r="R2">
+      <c r="S2">
         <v>184</v>
       </c>
-      <c r="S2">
+      <c r="T2">
         <v>935</v>
       </c>
-      <c r="T2">
+      <c r="U2">
         <v>0</v>
       </c>
-      <c r="U2" t="s">
-        <v>53</v>
+      <c r="V2" t="s">
+        <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C3" t="s">
         <v>13</v>
@@ -737,7 +746,7 @@
         <v>31</v>
       </c>
       <c r="H3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I3">
         <v>10</v>
@@ -746,48 +755,51 @@
         <v>50</v>
       </c>
       <c r="K3">
+        <v>100</v>
+      </c>
+      <c r="L3">
         <v>150</v>
       </c>
-      <c r="M3">
+      <c r="N3">
         <v>4</v>
       </c>
-      <c r="N3">
+      <c r="O3">
         <v>247</v>
       </c>
-      <c r="O3">
+      <c r="P3">
         <v>193</v>
       </c>
-      <c r="P3">
+      <c r="Q3">
         <v>47707</v>
       </c>
-      <c r="Q3">
+      <c r="R3">
         <v>247</v>
       </c>
-      <c r="R3">
+      <c r="S3">
         <v>914</v>
       </c>
-      <c r="S3">
+      <c r="T3">
         <v>8227</v>
       </c>
-      <c r="T3">
+      <c r="U3">
         <v>0</v>
       </c>
-      <c r="U3" t="s">
-        <v>54</v>
+      <c r="V3" t="s">
+        <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="C4" t="s">
         <v>14</v>
       </c>
       <c r="D4" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="E4" t="s">
         <v>26</v>
@@ -796,10 +808,7 @@
         <v>32</v>
       </c>
       <c r="H4" t="s">
-        <v>38</v>
-      </c>
-      <c r="I4">
-        <v>80</v>
+        <v>37</v>
       </c>
       <c r="J4">
         <v>60</v>
@@ -811,45 +820,48 @@
         <v>20</v>
       </c>
       <c r="M4">
+        <v>10</v>
+      </c>
+      <c r="N4">
         <v>2</v>
       </c>
-      <c r="N4">
+      <c r="O4">
         <v>42</v>
       </c>
-      <c r="O4">
+      <c r="P4">
         <v>190</v>
       </c>
-      <c r="P4">
+      <c r="Q4">
         <v>8141</v>
       </c>
-      <c r="Q4">
+      <c r="R4">
         <v>42</v>
       </c>
-      <c r="R4">
+      <c r="S4">
         <v>27</v>
       </c>
-      <c r="S4">
+      <c r="T4">
         <v>120</v>
       </c>
-      <c r="T4">
+      <c r="U4">
         <v>0</v>
       </c>
-      <c r="U4" t="s">
-        <v>55</v>
+      <c r="V4" t="s">
+        <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="C5" t="s">
         <v>15</v>
       </c>
       <c r="D5" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="E5" t="s">
         <v>26</v>
@@ -858,10 +870,7 @@
         <v>32</v>
       </c>
       <c r="H5" t="s">
-        <v>38</v>
-      </c>
-      <c r="I5">
-        <v>80</v>
+        <v>37</v>
       </c>
       <c r="J5">
         <v>60</v>
@@ -873,45 +882,48 @@
         <v>20</v>
       </c>
       <c r="M5">
+        <v>10</v>
+      </c>
+      <c r="N5">
         <v>3</v>
       </c>
-      <c r="N5">
+      <c r="O5">
         <v>36</v>
       </c>
-      <c r="O5">
+      <c r="P5">
         <v>190</v>
       </c>
-      <c r="P5">
+      <c r="Q5">
         <v>6914</v>
       </c>
-      <c r="Q5">
+      <c r="R5">
         <v>36</v>
       </c>
-      <c r="R5">
+      <c r="S5">
         <v>26</v>
       </c>
-      <c r="S5">
+      <c r="T5">
         <v>118</v>
       </c>
-      <c r="T5">
+      <c r="U5">
         <v>0</v>
       </c>
-      <c r="U5" t="s">
-        <v>56</v>
+      <c r="V5" t="s">
+        <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="C6" t="s">
         <v>16</v>
       </c>
       <c r="D6" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="E6" t="s">
         <v>27</v>
@@ -920,10 +932,7 @@
         <v>33</v>
       </c>
       <c r="H6" t="s">
-        <v>38</v>
-      </c>
-      <c r="I6">
-        <v>160</v>
+        <v>37</v>
       </c>
       <c r="J6">
         <v>120</v>
@@ -935,45 +944,48 @@
         <v>40</v>
       </c>
       <c r="M6">
+        <v>20</v>
+      </c>
+      <c r="N6">
         <v>2</v>
       </c>
-      <c r="N6">
+      <c r="O6">
         <v>120</v>
       </c>
-      <c r="O6">
+      <c r="P6">
         <v>186</v>
       </c>
-      <c r="P6">
+      <c r="Q6">
         <v>22460</v>
       </c>
-      <c r="Q6">
+      <c r="R6">
         <v>120</v>
       </c>
-      <c r="R6">
+      <c r="S6">
         <v>105</v>
       </c>
-      <c r="S6">
+      <c r="T6">
         <v>495</v>
       </c>
-      <c r="T6">
+      <c r="U6">
         <v>28</v>
       </c>
-      <c r="U6" t="s">
+      <c r="V6" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="C7" t="s">
         <v>17</v>
       </c>
       <c r="D7" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="E7" t="s">
         <v>28</v>
@@ -982,7 +994,7 @@
         <v>34</v>
       </c>
       <c r="H7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I7">
         <v>3</v>
@@ -993,40 +1005,43 @@
       <c r="K7">
         <v>20</v>
       </c>
-      <c r="M7">
+      <c r="L7">
+        <v>30</v>
+      </c>
+      <c r="N7">
         <v>2</v>
       </c>
-      <c r="N7">
+      <c r="O7">
         <v>8</v>
       </c>
-      <c r="O7">
+      <c r="P7">
         <v>51</v>
       </c>
-      <c r="P7">
+      <c r="Q7">
         <v>414</v>
       </c>
-      <c r="Q7">
+      <c r="R7">
         <v>8</v>
       </c>
-      <c r="R7">
+      <c r="S7">
         <v>10</v>
       </c>
-      <c r="S7">
+      <c r="T7">
         <v>42</v>
       </c>
-      <c r="T7">
+      <c r="U7">
         <v>0</v>
       </c>
-      <c r="U7" t="s">
-        <v>57</v>
+      <c r="V7" t="s">
+        <v>51</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="C8" t="s">
         <v>18</v>
@@ -1041,10 +1056,7 @@
         <v>34</v>
       </c>
       <c r="H8" t="s">
-        <v>38</v>
-      </c>
-      <c r="I8">
-        <v>100</v>
+        <v>37</v>
       </c>
       <c r="J8">
         <v>75</v>
@@ -1053,42 +1065,45 @@
         <v>50</v>
       </c>
       <c r="L8">
+        <v>25</v>
+      </c>
+      <c r="M8">
         <v>10</v>
       </c>
-      <c r="M8">
+      <c r="N8">
         <v>3</v>
       </c>
-      <c r="N8">
+      <c r="O8">
         <v>15</v>
       </c>
-      <c r="O8">
+      <c r="P8">
         <v>48</v>
       </c>
-      <c r="P8">
+      <c r="Q8">
         <v>749</v>
       </c>
-      <c r="Q8">
+      <c r="R8">
         <v>15</v>
       </c>
-      <c r="R8">
+      <c r="S8">
         <v>26</v>
       </c>
-      <c r="S8">
+      <c r="T8">
         <v>167</v>
       </c>
-      <c r="T8">
+      <c r="U8">
         <v>0</v>
       </c>
-      <c r="U8" t="s">
-        <v>58</v>
+      <c r="V8" t="s">
+        <v>52</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C9" t="s">
         <v>19</v>
@@ -1102,6 +1117,9 @@
       <c r="F9" t="s">
         <v>34</v>
       </c>
+      <c r="H9" t="s">
+        <v>36</v>
+      </c>
       <c r="I9">
         <v>1</v>
       </c>
@@ -1111,40 +1129,43 @@
       <c r="K9">
         <v>25</v>
       </c>
-      <c r="M9">
+      <c r="L9">
+        <v>50</v>
+      </c>
+      <c r="N9">
         <v>3</v>
       </c>
-      <c r="N9">
+      <c r="O9">
         <v>19</v>
       </c>
-      <c r="O9">
+      <c r="P9">
         <v>7</v>
       </c>
-      <c r="P9">
+      <c r="Q9">
         <v>133</v>
       </c>
-      <c r="Q9">
+      <c r="R9">
         <v>19</v>
       </c>
-      <c r="R9">
+      <c r="S9">
         <v>12</v>
       </c>
-      <c r="S9">
+      <c r="T9">
         <v>40</v>
       </c>
-      <c r="T9">
+      <c r="U9">
         <v>0</v>
       </c>
-      <c r="U9" t="s">
-        <v>59</v>
+      <c r="V9" t="s">
+        <v>53</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C10" t="s">
         <v>20</v>
@@ -1158,6 +1179,9 @@
       <c r="F10" t="s">
         <v>34</v>
       </c>
+      <c r="H10" t="s">
+        <v>36</v>
+      </c>
       <c r="I10">
         <v>10</v>
       </c>
@@ -1167,46 +1191,49 @@
       <c r="K10">
         <v>250</v>
       </c>
-      <c r="M10">
+      <c r="L10">
+        <v>500</v>
+      </c>
+      <c r="N10">
         <v>3</v>
       </c>
-      <c r="N10">
+      <c r="O10">
         <v>230</v>
       </c>
-      <c r="O10">
+      <c r="P10">
         <v>6</v>
       </c>
-      <c r="P10">
+      <c r="Q10">
         <v>1382</v>
       </c>
-      <c r="Q10">
+      <c r="R10">
         <v>230</v>
       </c>
-      <c r="R10">
+      <c r="S10">
         <v>337</v>
       </c>
-      <c r="S10">
+      <c r="T10">
         <v>979</v>
       </c>
-      <c r="T10">
+      <c r="U10">
         <v>30</v>
       </c>
-      <c r="U10" t="s">
-        <v>60</v>
+      <c r="V10" t="s">
+        <v>54</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C11" t="s">
         <v>21</v>
       </c>
       <c r="D11" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="E11" t="s">
         <v>26</v>
@@ -1214,6 +1241,9 @@
       <c r="F11" t="s">
         <v>31</v>
       </c>
+      <c r="H11" t="s">
+        <v>36</v>
+      </c>
       <c r="I11">
         <v>1</v>
       </c>
@@ -1223,32 +1253,35 @@
       <c r="K11">
         <v>3</v>
       </c>
-      <c r="M11">
+      <c r="L11">
+        <v>4</v>
+      </c>
+      <c r="N11">
         <v>2</v>
       </c>
-      <c r="N11">
+      <c r="O11">
         <v>1</v>
       </c>
-      <c r="O11">
+      <c r="P11">
         <v>191</v>
       </c>
-      <c r="P11">
+      <c r="Q11">
         <v>377</v>
-      </c>
-      <c r="Q11">
-        <v>1</v>
       </c>
       <c r="R11">
         <v>1</v>
       </c>
       <c r="S11">
+        <v>1</v>
+      </c>
+      <c r="T11">
         <v>19</v>
       </c>
-      <c r="T11">
+      <c r="U11">
         <v>0</v>
       </c>
-      <c r="U11" t="s">
-        <v>61</v>
+      <c r="V11" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>